<commit_message>
abstract schedule done + thesis description
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BME\Szakdoga\Szakdolgozat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3366BEBD-7865-4792-BF2F-D3941EBE9E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1D06A0-7045-400B-953E-C07EB880E5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3B9E0AFE-2744-466F-B98A-64987500D3E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>1. hét</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>Terv</t>
+  </si>
+  <si>
+    <t>Use Case Diagram, Wireframe, adatbázis drótháló</t>
+  </si>
+  <si>
+    <t>Adatbázis implementáció</t>
+  </si>
+  <si>
+    <t>Backend Implementáció</t>
+  </si>
+  <si>
+    <t>Frontend implementáció</t>
+  </si>
+  <si>
+    <t>Javítás, összeillesztési problémák feloldása</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Diagramok készítése, Dokumentáció, (0.Leadás) </t>
+  </si>
+  <si>
+    <t>Visszajelzések alapján javítás, Hivatalos leadás</t>
   </si>
 </sst>
 </file>
@@ -148,10 +169,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -469,13 +497,15 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="2" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -490,98 +520,120 @@
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>21</v>
+      </c>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>22</v>
+      </c>
       <c r="C15" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added notes to schedule
</commit_message>
<xml_diff>
--- a/Schedule.xlsx
+++ b/Schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BME\Szakdoga\Szakdolgozat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1D06A0-7045-400B-953E-C07EB880E5F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BF4C8BE-07CB-4502-9E22-6D5BCCFB893D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{3B9E0AFE-2744-466F-B98A-64987500D3E5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>1. hét</t>
   </si>
@@ -86,9 +86,6 @@
     <t>Terv</t>
   </si>
   <si>
-    <t>Use Case Diagram, Wireframe, adatbázis drótháló</t>
-  </si>
-  <si>
     <t>Adatbázis implementáció</t>
   </si>
   <si>
@@ -105,6 +102,21 @@
   </si>
   <si>
     <t>Visszajelzések alapján javítás, Hivatalos leadás</t>
+  </si>
+  <si>
+    <t>Funkcionális leírás, Use Case Diagram, Wireframe, adatbázis drótháló</t>
+  </si>
+  <si>
+    <t>Megjegyzés</t>
+  </si>
+  <si>
+    <t>xy</t>
+  </si>
+  <si>
+    <t>Hetente frissíteni kell az ütemezést, funkcionális leírás után tovább kell bontani az "xy" implementáció terveket</t>
+  </si>
+  <si>
+    <t>Dokumentáció szimultán készül a fejlesztés mellett, itt az erősebb fókuszt, befejezést jelenti</t>
   </si>
 </sst>
 </file>
@@ -171,14 +183,14 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,147 +506,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5438CF6-E54C-40AC-92B9-A0F653C746E1}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="51.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="2"/>
-    <col min="2" max="2" width="36.7109375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="2" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="36.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="89" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="3"/>
       <c r="C2" s="3"/>
     </row>
-    <row r="3" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
     </row>
-    <row r="4" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" s="1" t="s">
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1"/>
-    </row>
-    <row r="9" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="1"/>
-    </row>
-    <row r="10" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1"/>
-    </row>
-    <row r="11" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="1"/>
-    </row>
-    <row r="12" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1"/>
-    </row>
-    <row r="13" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C13" s="1"/>
-    </row>
-    <row r="14" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="2"/>
+      <c r="D14" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="1"/>
-    </row>
-    <row r="15" spans="1:3" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C15" s="1"/>
+      <c r="C15" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>